<commit_message>
Changed prints to logs Default to removing excel files Added requirements.txt
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\boletimtest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\~\my\git\data-to-excel-to-image\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>aluno</t>
   </si>
@@ -162,6 +162,15 @@
   </si>
   <si>
     <t>LUIZ GUSTAVO RAZZANO DE PONTES</t>
+  </si>
+  <si>
+    <t>dhadhkasjdas</t>
+  </si>
+  <si>
+    <t>dfdsfsdf</t>
+  </si>
+  <si>
+    <t>dsfsdfs</t>
   </si>
 </sst>
 </file>
@@ -540,15 +549,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR2"/>
+  <dimension ref="A1:AR5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="30" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="30" width="4" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="5.85546875" bestFit="1" customWidth="1"/>
@@ -825,6 +838,75 @@
       </c>
       <c r="AR2" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>345</v>
+      </c>
+      <c r="E4">
+        <v>35</v>
+      </c>
+      <c r="F4">
+        <v>34</v>
+      </c>
+      <c r="G4">
+        <v>45345</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>345</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="AN5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>